<commit_message>
fixed parsing bulk label data
</commit_message>
<xml_diff>
--- a/frontend/public/media/kemlabels-bulk-order-towa.xlsx
+++ b/frontend/public/media/kemlabels-bulk-order-towa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elber\Documents\GitHub\ShippingProject\backend\bulkOrders\tt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elber\Documents\GitHub\ShippingProject\frontend\public\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BED78B-EB4F-4E3E-966F-8E3C44FF19BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8939A24-F92D-41A5-BA9E-62F6ECC73333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10605" yWindow="2280" windowWidth="16470" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="2175" windowWidth="24795" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kemlabels-bulk-order-template" sheetId="1" r:id="rId1"/>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1493,7 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations xWindow="257" yWindow="264" count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Courier" prompt="Please select a courier" sqref="A1" xr:uid="{BC05BADB-F766-4E79-BCB6-8075CB7A0E72}">
-      <formula1>"USPS, UPSUSA, UPSCA"</formula1>
+      <formula1>"USPS, UPS USA, UPS CA"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Select YES or NO" promptTitle="Signature" prompt="Please select 'Yes' for signature." sqref="C1" xr:uid="{936E74DA-DDE8-40E6-8088-3041A2A45579}">
       <formula1>"YES, NO"</formula1>

</xml_diff>

<commit_message>
fixed bulk order names and courier assignments
</commit_message>
<xml_diff>
--- a/frontend/public/media/kemlabels-bulk-order-towa.xlsx
+++ b/frontend/public/media/kemlabels-bulk-order-towa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elber\Documents\GitHub\ShippingProject\frontend\public\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5798347C-F58D-42AB-BBD9-12215C4748C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0FDF54-2527-45A4-916F-C583AE245BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1950" windowWidth="24795" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>USPS</t>
   </si>
@@ -1056,10 +1056,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,218 +1275,6 @@
         <v>30</v>
       </c>
       <c r="T4" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>11706</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="1">
-        <v>78752</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>30</v>
-      </c>
-      <c r="R5" s="1">
-        <v>30</v>
-      </c>
-      <c r="S5" s="1">
-        <v>30</v>
-      </c>
-      <c r="T5" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1">
-        <v>11706</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="1">
-        <v>78752</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>30</v>
-      </c>
-      <c r="R6" s="1">
-        <v>30</v>
-      </c>
-      <c r="S6" s="1">
-        <v>30</v>
-      </c>
-      <c r="T6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1">
-        <v>11706</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="1">
-        <v>78752</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>30</v>
-      </c>
-      <c r="R7" s="1">
-        <v>30</v>
-      </c>
-      <c r="S7" s="1">
-        <v>30</v>
-      </c>
-      <c r="T7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="1">
-        <v>11706</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="1">
-        <v>78752</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>30</v>
-      </c>
-      <c r="R8" s="1">
-        <v>30</v>
-      </c>
-      <c r="S8" s="1">
-        <v>30</v>
-      </c>
-      <c r="T8" s="1">
         <v>50</v>
       </c>
     </row>

</xml_diff>